<commit_message>
update chart and figure
</commit_message>
<xml_diff>
--- a/Chart.xlsx
+++ b/Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a111111/Desktop/GitHub/StereotypicalSuggestions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EFBA0E7-BC65-D640-AD13-69E76DA4021E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81E031D-E0D3-BA44-90ED-0E299BD216D3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="860" windowWidth="27640" windowHeight="15600" xr2:uid="{D6802059-6949-DD4D-B097-75B627D03B95}"/>
+    <workbookView xWindow="780" yWindow="720" windowWidth="27640" windowHeight="15600" xr2:uid="{D6802059-6949-DD4D-B097-75B627D03B95}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -885,8 +885,69 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Person descriptors count</a:t>
+              <a:t>Person descriptors </a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>number</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>spotted</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+              <a:t>on</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+              <a:t>the</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+              <a:t>image</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+              <a:t>search</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+              <a:t>engine</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+              <a:t>search</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -3273,7 +3334,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>